<commit_message>
Additional documents were added for preparing manuscript
</commit_message>
<xml_diff>
--- a/Results/What-if scenarios effect.xlsx
+++ b/Results/What-if scenarios effect.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luxma\OneDrive\Documents\Cornell\Projects\MC Milk\MC-2020\Tim_ESL\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE2AC9F-3652-4895-B26C-B7E1AAE1BF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FAAB21-1C15-44D8-B45C-B9B99D980D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13515" yWindow="3705" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="2865" windowWidth="25230" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
   <si>
     <t>Base model</t>
   </si>
@@ -255,6 +255,24 @@
   </si>
   <si>
     <t>supercool</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>mean 1.8</t>
+  </si>
+  <si>
+    <t>censore at 4</t>
+  </si>
+  <si>
+    <t>transport T</t>
+  </si>
+  <si>
+    <t>transport t</t>
   </si>
 </sst>
 </file>
@@ -284,7 +302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +312,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -319,6 +343,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2A8D80-C843-4049-8104-466112E73759}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:AI30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +635,7 @@
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>63</v>
       </c>
@@ -618,7 +643,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -629,7 +654,7 @@
         <v>0.55300000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -648,7 +673,7 @@
         <v>0.19000000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -667,7 +692,7 @@
         <v>0.12600000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -686,7 +711,7 @@
         <v>0.17800000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -705,7 +730,7 @@
         <v>1.3000000000000012E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -724,7 +749,7 @@
         <v>2.4000000000000021E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -743,7 +768,7 @@
         <v>2.0000000000000018E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -762,7 +787,7 @@
         <v>1.0000000000000009E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -781,7 +806,7 @@
         <v>1.5000000000000013E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -798,6 +823,1417 @@
       <c r="E11">
         <f t="shared" si="1"/>
         <v>-1.8999999999999906E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <v>9</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>11</v>
+      </c>
+      <c r="L14">
+        <v>12</v>
+      </c>
+      <c r="M14">
+        <v>13</v>
+      </c>
+      <c r="N14">
+        <v>14</v>
+      </c>
+      <c r="O14">
+        <v>15</v>
+      </c>
+      <c r="P14">
+        <v>16</v>
+      </c>
+      <c r="Q14">
+        <v>17</v>
+      </c>
+      <c r="R14">
+        <v>18</v>
+      </c>
+      <c r="S14">
+        <v>19</v>
+      </c>
+      <c r="T14">
+        <v>20</v>
+      </c>
+      <c r="U14">
+        <v>21</v>
+      </c>
+      <c r="V14">
+        <v>22</v>
+      </c>
+      <c r="W14">
+        <v>23</v>
+      </c>
+      <c r="X14">
+        <v>24</v>
+      </c>
+      <c r="Y14">
+        <v>25</v>
+      </c>
+      <c r="Z14">
+        <v>26</v>
+      </c>
+      <c r="AA14">
+        <v>27</v>
+      </c>
+      <c r="AB14">
+        <v>28</v>
+      </c>
+      <c r="AC14">
+        <v>29</v>
+      </c>
+      <c r="AD14">
+        <v>30</v>
+      </c>
+      <c r="AE14">
+        <v>31</v>
+      </c>
+      <c r="AF14">
+        <v>32</v>
+      </c>
+      <c r="AG14">
+        <v>33</v>
+      </c>
+      <c r="AH14">
+        <v>34</v>
+      </c>
+      <c r="AI14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C15">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D15">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="E15">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.123</v>
+      </c>
+      <c r="G15">
+        <v>0.154</v>
+      </c>
+      <c r="H15">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="I15">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="J15">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="K15">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="L15">
+        <v>0.316</v>
+      </c>
+      <c r="M15">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="N15">
+        <v>0.38</v>
+      </c>
+      <c r="O15">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="P15">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="Q15">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="R15" s="4">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="S15">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="T15">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="U15">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="V15">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="W15">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="X15">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="Y15">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="Z15">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="AA15">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="AB15">
+        <v>0.67</v>
+      </c>
+      <c r="AC15">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="AD15">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="AE15">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="AF15">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="AG15">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="AH15">
+        <v>0.746</v>
+      </c>
+      <c r="AI15">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1E-3</v>
+      </c>
+      <c r="D16">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E16">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F16">
+        <v>2.7E-2</v>
+      </c>
+      <c r="G16">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H16">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="I16">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J16">
+        <v>0.108</v>
+      </c>
+      <c r="K16">
+        <v>0.13</v>
+      </c>
+      <c r="L16">
+        <v>0.15</v>
+      </c>
+      <c r="M16">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="N16">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="O16">
+        <v>0.221</v>
+      </c>
+      <c r="P16">
+        <v>0.249</v>
+      </c>
+      <c r="Q16">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="R16">
+        <v>0.307</v>
+      </c>
+      <c r="S16">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="T16">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="U16">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="V16">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="W16">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="X16">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="Y16">
+        <v>0.443</v>
+      </c>
+      <c r="Z16">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="AB16">
+        <v>0.501</v>
+      </c>
+      <c r="AC16">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="AD16">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="AE16">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="AF16">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="AG16">
+        <v>0.59</v>
+      </c>
+      <c r="AH16">
+        <v>0.6</v>
+      </c>
+      <c r="AI16">
+        <v>0.61099999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C17">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D17">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E17">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F17">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="G17">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H17">
+        <v>0.09</v>
+      </c>
+      <c r="I17">
+        <v>0.121</v>
+      </c>
+      <c r="J17">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="K17">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="L17">
+        <v>0.191</v>
+      </c>
+      <c r="M17">
+        <v>0.217</v>
+      </c>
+      <c r="N17">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="O17">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="P17">
+        <v>0.311</v>
+      </c>
+      <c r="Q17">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="R17">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="S17">
+        <v>0.378</v>
+      </c>
+      <c r="T17">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="U17">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="V17">
+        <v>0.45</v>
+      </c>
+      <c r="W17">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="X17" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="Y17">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="Z17">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="AA17">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="AB17">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="AC17">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AD17">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="AE17">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="AF17">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="AG17">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="AH17">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="AI17">
+        <v>0.66600000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1E-3</v>
+      </c>
+      <c r="D18">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E18">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F18">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="G18">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="H18">
+        <v>0.06</v>
+      </c>
+      <c r="I18">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="J18">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="K18">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="L18">
+        <v>0.159</v>
+      </c>
+      <c r="M18">
+        <v>0.185</v>
+      </c>
+      <c r="N18">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="O18">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="P18">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="Q18">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="R18">
+        <v>0.317</v>
+      </c>
+      <c r="S18">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="T18">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="U18">
+        <v>0.375</v>
+      </c>
+      <c r="V18">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="W18">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="X18">
+        <v>0.438</v>
+      </c>
+      <c r="Y18">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="Z18">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="AA18" s="4">
+        <v>0.498</v>
+      </c>
+      <c r="AB18">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="AC18">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="AD18">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="AE18">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="AF18">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="AG18">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="AH18">
+        <v>0.61</v>
+      </c>
+      <c r="AI18">
+        <v>0.626</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C19">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D19">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="E19">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F19">
+        <v>0.107</v>
+      </c>
+      <c r="G19">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="H19">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="I19">
+        <v>0.2</v>
+      </c>
+      <c r="J19">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="K19">
+        <v>0.27</v>
+      </c>
+      <c r="L19">
+        <v>0.3</v>
+      </c>
+      <c r="M19">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="N19">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="O19">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="P19">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="Q19">
+        <v>0.442</v>
+      </c>
+      <c r="R19">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="S19" s="4">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="T19">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="U19">
+        <v>0.54</v>
+      </c>
+      <c r="V19">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="W19">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="X19">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="Y19">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="Z19">
+        <v>0.629</v>
+      </c>
+      <c r="AA19">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AB19">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="AC19">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="AD19">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="AE19">
+        <v>0.7</v>
+      </c>
+      <c r="AF19">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="AG19">
+        <v>0.72</v>
+      </c>
+      <c r="AH19">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="AI19">
+        <v>0.73599999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C20">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D20">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E20">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F20">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="G20">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H20">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="I20">
+        <v>0.19</v>
+      </c>
+      <c r="J20">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K20">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="L20">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="M20">
+        <v>0.317</v>
+      </c>
+      <c r="N20">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="O20">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="P20">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="Q20">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="R20">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="S20">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="T20" s="4">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="U20">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="V20">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="W20">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="X20">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="Y20">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="Z20">
+        <v>0.62</v>
+      </c>
+      <c r="AA20">
+        <v>0.629</v>
+      </c>
+      <c r="AB20">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="AC20">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="AD20">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="AE20">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="AF20">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="AG20">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="AH20">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="AI20">
+        <v>0.72599999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C21">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D21">
+        <v>0.06</v>
+      </c>
+      <c r="E21">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="F21">
+        <v>0.123</v>
+      </c>
+      <c r="G21">
+        <v>0.152</v>
+      </c>
+      <c r="H21">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="I21">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="J21">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="K21">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="L21">
+        <v>0.315</v>
+      </c>
+      <c r="M21">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="N21">
+        <v>0.379</v>
+      </c>
+      <c r="O21">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="P21">
+        <v>0.43</v>
+      </c>
+      <c r="Q21">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="R21" s="4">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="S21">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="T21">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="U21">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="V21">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="W21">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="X21">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="Y21">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="Z21">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="AA21">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="AB21">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="AC21">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="AD21">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="AE21">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="AF21">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="AG21">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="AH21">
+        <v>0.746</v>
+      </c>
+      <c r="AI21">
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="C22">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D22">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="E22">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F22">
+        <v>0.115</v>
+      </c>
+      <c r="G22">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="H22">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="I22">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="J22">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="K22">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="L22">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="M22">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="N22">
+        <v>0.375</v>
+      </c>
+      <c r="O22">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="P22">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="Q22">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="R22">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="S22" s="4">
+        <v>0.499</v>
+      </c>
+      <c r="T22">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="U22">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="V22">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="W22">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="X22">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="Y22">
+        <v>0.628</v>
+      </c>
+      <c r="Z22">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="AA22">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="AB22">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="AC22">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="AD22">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="AE22">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="AF22">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="AG22">
+        <v>0.73</v>
+      </c>
+      <c r="AH22">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="AI22">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C23">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D23">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E23">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="F23">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="G23">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="H23">
+        <v>0.153</v>
+      </c>
+      <c r="I23">
+        <v>0.188</v>
+      </c>
+      <c r="J23">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K23">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="L23">
+        <v>0.3</v>
+      </c>
+      <c r="M23">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="N23">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="O23">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="P23">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="Q23">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="R23">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="S23" s="4">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="T23">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="U23">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="V23">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="W23">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="X23">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="Y23">
+        <v>0.63</v>
+      </c>
+      <c r="Z23">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AA23">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="AB23">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="AC23">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="AD23">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="AE23">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="AF23">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="AG23">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="AH23">
+        <v>0.749</v>
+      </c>
+      <c r="AI23">
+        <v>0.75900000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C24">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.05</v>
+      </c>
+      <c r="E24">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F24">
+        <v>0.11</v>
+      </c>
+      <c r="G24">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="H24">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="I24">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="J24">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="K24">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="L24">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="M24">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="N24">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="O24">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="P24">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="Q24">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="R24" s="4">
+        <v>0.49</v>
+      </c>
+      <c r="S24">
+        <v>0.52</v>
+      </c>
+      <c r="T24">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="U24">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="V24">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="W24">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="X24">
+        <v>0.625</v>
+      </c>
+      <c r="Y24">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="Z24">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="AA24">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="AB24">
+        <v>0.68</v>
+      </c>
+      <c r="AC24">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="AD24">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="AE24">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="AF24">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="AG24">
+        <v>0.746</v>
+      </c>
+      <c r="AH24">
+        <v>0.75</v>
+      </c>
+      <c r="AI24">
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E25">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F25">
+        <v>0.03</v>
+      </c>
+      <c r="G25">
+        <v>5.5E-2</v>
+      </c>
+      <c r="H25">
+        <v>9.4E-2</v>
+      </c>
+      <c r="I25">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="J25">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="K25">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="L25">
+        <v>0.2</v>
+      </c>
+      <c r="M25">
+        <v>0.23</v>
+      </c>
+      <c r="N25">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="O25">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="P25">
+        <v>0.309</v>
+      </c>
+      <c r="Q25">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="R25">
+        <v>0.371</v>
+      </c>
+      <c r="S25">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="T25">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="U25">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="V25">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="W25" s="4">
+        <v>0.497</v>
+      </c>
+      <c r="X25">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="Y25">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="Z25">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="AA25">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="AB25">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="AC25">
+        <v>0.59</v>
+      </c>
+      <c r="AD25">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="AE25">
+        <v>0.62</v>
+      </c>
+      <c r="AF25">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="AG25">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="AH25">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="AI25">
+        <v>0.67100000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C26">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D26">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E26">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="F26">
+        <v>7.8E-2</v>
+      </c>
+      <c r="G26">
+        <v>0.111</v>
+      </c>
+      <c r="H26">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="I26">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="J26">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="K26">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="L26">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="M26">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="N26">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="O26">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="P26">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="Q26">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="R26">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="S26">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="T26" s="4">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="U26">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="V26">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="W26">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="X26">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="Y26">
+        <v>0.6</v>
+      </c>
+      <c r="Z26">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="AA26">
+        <v>0.625</v>
+      </c>
+      <c r="AB26">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="AC26">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="AD26">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="AE26">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AF26">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="AG26">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="AH26">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="AI26">
+        <v>0.72599999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <f>N15-N25</f>
+        <v>0.124</v>
+      </c>
+      <c r="U29">
+        <f>U15-U25</f>
+        <v>0.10000000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <f>N15-N26</f>
+        <v>5.099999999999999E-2</v>
+      </c>
+      <c r="U30">
+        <f>U15-U26</f>
+        <v>3.5000000000000031E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>